<commit_message>
Corrección de links a código .qmd desde calendario.
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (Maestral)/Documentos/Clases/UC - Web scraping 2023/web_scraping_soc40XX_2023/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0FCD3D-B16B-7F49-9C4D-7E647381C81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55F88EA-2BD2-C14E-B608-C7389EE54424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34560" yWindow="1240" windowWidth="32600" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
@@ -104,36 +104,6 @@
     <t>Propuesta TF</t>
   </si>
   <si>
-    <t>[Slides](slides/class_1/class_1#1) [.Rmd](slides/class_1/class_1.Rmd)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_2/class_2#1) [.Rmd](slides/class_2/class_2.Rmd) [.R](slides/class_2/class_2_taller.R)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_3/class_3#1) [.Rmd](slides/class_3/class_3.Rmd)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_5/class_5#1) [.Rmd](slides/class_5/class_5.Rmd)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_4/class_4#1) [.Rmd](slides/class_4/class_4.Rmd) [.R](slides/class_4/class_4_taller.R)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_6/class_6#1) [.Rmd](slides/class_6/class_6.Rmd) [.R](slides/class_6/class_6_taller.R)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_7/class_7#1) [.Rmd](slides/class_7/class_7.Rmd)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_8/class_8#1) [.Rmd](slides/class_8/class_8.Rmd)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_9/class_9#1) [.Rmd](slides/class_9/class_9.Rmd)</t>
-  </si>
-  <si>
-    <t>[Slides](slides/class_10/class_10#1) [.Rmd](slides/class_10/class_10.Rmd)</t>
-  </si>
-  <si>
     <t>Uso headless browser: chromote</t>
   </si>
   <si>
@@ -150,6 +120,36 @@
   </si>
   <si>
     <t>Presentación trabajo final</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_1/class_1#1) [.qmd](slides/class_1/class_1.qmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_2/class_2#1) [.qmd](slides/class_2/class_2.qmd) [.R](slides/class_2/class_2_taller.R)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_3/class_3#1) [.qmd](slides/class_3/class_3.qmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_4/class_4#1) [.qmd](slides/class_4/class_4.qmd) [.R](slides/class_4/class_4_taller.R)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_5/class_5#1) [.qmd](slides/class_5/class_5.qmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_6/class_6#1) [.qmd](slides/class_6/class_6.qmd) [.R](slides/class_6/class_6_taller.R)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_7/class_7#1) [.qmd](slides/class_7/class_7.qmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_8/class_8#1) [.qmd](slides/class_8/class_8.qmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_9/class_9#1) [.qmd](slides/class_9/class_9.qmd)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_10/class_10#1) [.qmd](slides/class_10/class_10.qmd)</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -592,7 +592,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -676,7 +676,7 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -728,10 +728,10 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -746,10 +746,10 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -767,7 +767,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -835,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -843,7 +843,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -859,7 +859,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -867,7 +867,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -875,7 +875,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Actualización links en README
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (Maestral)/Documentos/Clases/UC - Web scraping 2023/web_scraping_soc40XX_2023/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FBE423-596E-FC41-9A53-C9C575296DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0485FC61-FAC2-FC48-8D10-43F9A5388D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>tipo</t>
   </si>
@@ -519,7 +519,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,6 +612,9 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -632,6 +635,9 @@
       </c>
       <c r="F5" t="s">
         <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -782,7 +788,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B5" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Links a Clase 9 en tabla.
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10702"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (DESUC)/Documentos/Clases/UC - Web scraping 2023/web_scraping_soc40XX_2023/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F699D34-F80B-1B4D-8633-8893BE4B9517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FE87D4-2F0D-964A-94AE-73DDABB2E848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="1440" windowWidth="34560" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
+    <workbookView xWindow="35860" yWindow="1240" windowWidth="34560" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
   <si>
     <t>tipo</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Web Scraping avanzado</t>
   </si>
   <si>
-    <t>C3 (20%)</t>
-  </si>
-  <si>
     <t>Propuesta TF</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>[C2 (20%)](homework/c_2.html)</t>
+  </si>
+  <si>
+    <t>[C3 (20%)](homework/c_3.html)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_8/class_8#1) [.qmd](slides/class_8/class_8.qmd) [.R](slides/class_8/class_8_taller.R)</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,7 +574,7 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -592,7 +595,7 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -613,7 +616,7 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -634,10 +637,10 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -658,7 +661,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -679,16 +682,16 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -708,10 +711,10 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -731,7 +734,7 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -746,10 +749,13 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -764,13 +770,13 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -785,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -829,7 +835,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -837,7 +843,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -845,7 +851,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -853,7 +859,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -861,7 +867,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -869,7 +875,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -877,7 +883,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -885,7 +891,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -893,7 +899,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Dirección slides clase 11.
</commit_message>
<xml_diff>
--- a/files/02-calendario.xlsx
+++ b/files/02-calendario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10702"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caayala/Dropbox (DESUC)/Documentos/Clases/UC - Web scraping 2023/web_scraping_soc40XX_2023/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFD0C97-2FA4-7C4D-914F-FB03D810F196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D63749-A588-D84D-9CB3-B377ABE9DA80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
+    <workbookView xWindow="34560" yWindow="1240" windowWidth="38400" windowHeight="21100" xr2:uid="{C0FA5A6A-09BB-DF4A-BC0A-ED4474CC6351}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,10 +155,10 @@
     <t>[Slides](slides/class_8/class_8#1) [.qmd](slides/class_8/class_8.qmd) [.R](slides/class_8/class_8_taller.R)</t>
   </si>
   <si>
-    <t>[Slides](slides/class_11/class_10#1) [.qmd](slides/class_11/class_11.qmd)</t>
-  </si>
-  <si>
     <t>[`usethis`](https://usethis.r-lib.org), [GitHub Actions](https://docs.github.com/en/actions)</t>
+  </si>
+  <si>
+    <t>[Slides](slides/class_11/class_11#1) [.qmd](slides/class_11/class_11.qmd)</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -803,10 +803,10 @@
         <v>24</v>
       </c>
       <c r="E13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
         <v>40</v>
-      </c>
-      <c r="G13" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>